<commit_message>
@add common variable and add data in excel sheet
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/FieldSetComponentDataSheet.xlsx
+++ b/FieldSetComponentDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E138004-E095-4116-8F94-DA7041BAB3A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D601D023-C260-48B0-93A9-13D6D2F9D9E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -103,6 +103,48 @@
   </si>
   <si>
     <t>Phone</t>
+  </si>
+  <si>
+    <t>FS1</t>
+  </si>
+  <si>
+    <t>FS2</t>
+  </si>
+  <si>
+    <t>FS3</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>9876546789</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Ins1</t>
+  </si>
+  <si>
+    <t>AIG Sun life</t>
+  </si>
+  <si>
+    <t>Contact Deal</t>
+  </si>
+  <si>
+    <t>Deal1</t>
+  </si>
+  <si>
+    <t>Deal Received</t>
+  </si>
+  <si>
+    <t>Test David</t>
+  </si>
+  <si>
+    <t>AIG Sun Life</t>
   </si>
 </sst>
 </file>
@@ -181,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -198,6 +240,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,73 +522,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -557,10 +613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{039D01EB-1016-4148-939A-D18F1C4E638F}">
-  <dimension ref="A1:ALO1"/>
+  <dimension ref="A1:ALO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1581,6 +1637,14 @@
       <c r="ALN1" s="5"/>
       <c r="ALO1" s="5"/>
     </row>
+    <row r="2" spans="1:1003" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1588,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E897D9-152C-4D67-A3B8-1E6680A82519}">
-  <dimension ref="A1:ALR1"/>
+  <dimension ref="A1:ALR2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,7 +1664,7 @@
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
@@ -2623,6 +2687,23 @@
       <c r="ALQ1" s="5"/>
       <c r="ALR1" s="5"/>
     </row>
+    <row r="2" spans="1:1006" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2630,10 +2711,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C36F35-936B-433C-9C73-2ED89ECCFD09}">
-  <dimension ref="A1:AML1"/>
+  <dimension ref="A1:AML2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2641,7 +2722,7 @@
     <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3686,6 +3767,26 @@
       <c r="AMK1" s="6"/>
       <c r="AML1" s="6"/>
     </row>
+    <row r="2" spans="1:1026" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
@add tc005 and tc006
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/FieldSetComponentDataSheet.xlsx
+++ b/FieldSetComponentDataSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E2075A-3D39-4FF0-9D07-05587F98CA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBFC648-F755-48DA-AD31-058EB3F4AF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FieldSet" sheetId="1" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2725,7 +2725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C36F35-936B-433C-9C73-2ED89ECCFD09}">
   <dimension ref="A1:AML2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
@add tc009 and method changepositionofFieldInCreatedFieldSet
Signed-off-by: Ankit Jaiswal <ajaiswal@navatargroup.com>
</commit_message>
<xml_diff>
--- a/FieldSetComponentDataSheet.xlsx
+++ b/FieldSetComponentDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBFC648-F755-48DA-AD31-058EB3F4AF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A297E3-6538-4238-91FB-FDC34121C21F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,24 +42,15 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Contact Detail - FSet1</t>
-  </si>
-  <si>
     <t>On Contact Page</t>
   </si>
   <si>
     <t>Fields_Name</t>
   </si>
   <si>
-    <t>Contact Detail - FSet2</t>
-  </si>
-  <si>
     <t>Deal</t>
   </si>
   <si>
-    <t>Deal Detail - FSet1</t>
-  </si>
-  <si>
     <t>On Deal Page</t>
   </si>
   <si>
@@ -148,6 +139,15 @@
   </si>
   <si>
     <t>navatariptesting+27971@gmail.com</t>
+  </si>
+  <si>
+    <t>Contact_Detail_FSet1</t>
+  </si>
+  <si>
+    <t>Contact_Detail_FSet2</t>
+  </si>
+  <si>
+    <t>Deal_Detail_FSet1</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +542,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -554,58 +554,58 @@
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -631,13 +631,13 @@
   <sheetData>
     <row r="1" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="2" spans="1:1003" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1676,25 +1676,25 @@
   <sheetData>
     <row r="1" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -2698,22 +2698,22 @@
     </row>
     <row r="2" spans="1:1006" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -2741,25 +2741,25 @@
   <sheetData>
     <row r="1" spans="1:1026" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -3783,22 +3783,22 @@
     </row>
     <row r="2" spans="1:1026" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>36</v>
-      </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tc010 and tc011
</commit_message>
<xml_diff>
--- a/FieldSetComponentDataSheet.xlsx
+++ b/FieldSetComponentDataSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Navatar_Projects\einstein-code-version-2-pe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A297E3-6538-4238-91FB-FDC34121C21F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DA39E7-0A30-476C-A3BB-B53FC5469B9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Entities" sheetId="3" r:id="rId2"/>
     <sheet name="Contacts" sheetId="2" r:id="rId3"/>
     <sheet name="Deal" sheetId="4" r:id="rId4"/>
+    <sheet name="FieldComponent" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>NameSpace_PreFix</t>
   </si>
@@ -148,6 +149,39 @@
   </si>
   <si>
     <t>Deal_Detail_FSet1</t>
+  </si>
+  <si>
+    <t>FC1</t>
+  </si>
+  <si>
+    <t>Title ^@^&amp;!^^&amp; Title ^&amp;^&amp;@^&amp;!^</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>Field_Label</t>
+  </si>
+  <si>
+    <t>Field_Type</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>FieldLabel_SubString</t>
+  </si>
+  <si>
+    <t>Title ^@</t>
+  </si>
+  <si>
+    <t>ExtraFieldsName</t>
+  </si>
+  <si>
+    <t>Contact&lt;break&gt;Relationship Type&lt;break&gt;Candidate Notes&lt;break&gt;Do Not Call&lt;break&gt;Email 2&lt;break&gt;Fax&lt;break&gt;Other City&lt;break&gt;Individual&lt;break&gt;Reports To&lt;break&gt;Relationship Owners&lt;break&gt;Average Deal Quality Score&lt;break&gt;Assistant&lt;break&gt;Total Deals Shown&lt;break&gt;Tier&lt;break&gt;Lead Source&lt;break&gt;Department&lt;break&gt;Contact Type&lt;break&gt;Email Opt Out&lt;break&gt;Created By&lt;break&gt;Office Location&lt;break&gt;Created Date&lt;break&gt;Mailing City&lt;break&gt;Owner&lt;break&gt;Asst. Phone&lt;break&gt;Description&lt;break&gt;Primary Contact&lt;break&gt;Birthdate&lt;break&gt;Source&lt;break&gt;Contact Referral Source&lt;break&gt;Region&lt;break&gt;Potential Candidate&lt;break&gt;Phone 2&lt;break&gt;Photo URL&lt;break&gt;Other Street&lt;break&gt;Last Touch Point&lt;break&gt;Candidate Role&lt;break&gt;Other Latitude&lt;break&gt;Candidate Status&lt;break&gt;Mailing Street&lt;break&gt;Industry&lt;break&gt;Last Stay-in-Touch Request Date&lt;break&gt;Mailing Country&lt;break&gt;Last Referenced Date&lt;break&gt;External System ID&lt;break&gt;Last Name&lt;break&gt;Email 3&lt;break&gt;Fax Opt Out</t>
   </si>
 </sst>
 </file>
@@ -525,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +571,11 @@
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="77.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -556,8 +591,11 @@
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -573,8 +611,11 @@
       <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -591,7 +632,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3804,4 +3845,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B8B9A0-4A66-4C6E-B716-5700689FB494}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>